<commit_message>
added overload calculation for scale max added winch specs image
</commit_message>
<xml_diff>
--- a/Cost Estimation.xlsx
+++ b/Cost Estimation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacob/Documents/Visual Studio Code/Crowley-SDA-Church/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDA7931-7EFF-E247-BDE1-87AB5E3E37A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E320CD8-CA15-4A44-9918-FAA3976989C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34860" yWindow="500" windowWidth="16340" windowHeight="12980" xr2:uid="{85812CC2-4E4D-D948-9692-9D663EF942EB}"/>
+    <workbookView xWindow="1120" yWindow="880" windowWidth="34880" windowHeight="22500" xr2:uid="{85812CC2-4E4D-D948-9692-9D663EF942EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Item</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Purpose</t>
   </si>
   <si>
-    <t>Arduino</t>
-  </si>
-  <si>
     <t>Hardware</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t xml:space="preserve">✅     </t>
+  </si>
+  <si>
+    <t>Signal Conditioner</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="B4:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,42 +504,34 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <f>50-25</f>
+        <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -548,7 +540,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>50</v>
@@ -557,39 +549,42 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>50</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>55</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>200</v>
@@ -598,25 +593,37 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>50</v>
       </c>
+      <c r="D13" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>65</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
-        <v>30</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>45</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
@@ -637,7 +644,7 @@
     <row r="21" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C21">
         <f>SUM(C5:C20)</f>
-        <v>515</v>
+        <v>555</v>
       </c>
       <c r="F21" s="2"/>
     </row>

</xml_diff>

<commit_message>
remove FreeRTOS, update Cost Estimation,\ DFRobot RS485 Adapter, working LED blink project
</commit_message>
<xml_diff>
--- a/Cost Estimation.xlsx
+++ b/Cost Estimation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacob/Documents/Visual Studio Code/Crowley-SDA-Church/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E320CD8-CA15-4A44-9918-FAA3976989C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A4DA42-1EA5-504A-AE19-A0AD9EEBF182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="880" windowWidth="34880" windowHeight="22500" xr2:uid="{85812CC2-4E4D-D948-9692-9D663EF942EB}"/>
+    <workbookView xWindow="1320" yWindow="880" windowWidth="34680" windowHeight="22500" xr2:uid="{85812CC2-4E4D-D948-9692-9D663EF942EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Item</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>display</t>
-  </si>
-  <si>
-    <t>https://www.buydisplay.com/4-3-lcd-touch-screen-module-display-tft-ssd1963-controller-mcu?srsltid=AfmBOop8-uBfpCnzvIvkKWw28VsWtkl-nTbRvMLGql4BeKHfGfiivKTA</t>
   </si>
   <si>
     <t>STM nucleo 2x</t>
@@ -484,7 +481,7 @@
   <dimension ref="B4:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>2</v>
@@ -518,14 +515,14 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <f>50-25</f>
         <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -566,7 +563,7 @@
         <v>55</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -578,7 +575,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -599,7 +596,7 @@
         <v>50</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -608,21 +605,22 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>65</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>45</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -644,7 +642,7 @@
     <row r="21" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C21">
         <f>SUM(C5:C20)</f>
-        <v>555</v>
+        <v>690</v>
       </c>
       <c r="F21" s="2"/>
     </row>

</xml_diff>